<commit_message>
added an example of filling based on an array/slice
</commit_message>
<xml_diff>
--- a/example/result.xlsx
+++ b/example/result.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Report 05.01.2023 in 00:15:35</t>
+    <t>Report 07.01.2023 in 09:30:53</t>
   </si>
   <si>
     <t/>
@@ -53,7 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -64,8 +64,9 @@
     <font>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="0"/>
+      <charset val="0"/>
+      <color rgb="FF000000"/>
       <b/>
     </font>
     <font>
@@ -77,23 +78,32 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="0"/>
+      <charset val="0"/>
       <color rgb="FFF10D0C"/>
       <b/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="0"/>
+      <charset val="0"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="0"/>
+      <charset val="0"/>
+      <color rgb="FF000000"/>
       <b/>
+    </font>
+    <font>
+      <sz val="0"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="0"/>
+      <color rgb="FF000000"/>
     </font>
   </fonts>
   <fills count="5">
@@ -106,7 +116,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5EB91E"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF5EB91E"/>
       </patternFill>
     </fill>
     <fill>
@@ -115,7 +125,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
   </fills>
@@ -133,10 +143,18 @@
       <bottom style="none"/>
     </border>
     <border>
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -144,13 +162,16 @@
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="2" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -171,6 +192,9 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="1" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="0" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -501,114 +525,171 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="18.34"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.52"/>
+    <col max="4" min="1" style="0" width="18.38"/>
+    <col max="6" min="5" style="0" width="11.5"/>
+    <col max="26" min="7" style="0" width="8.63"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.35" customHeight="true">
+    <row r="1" ht="12.75" customHeight="true">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" ht="12.8" customHeight="true">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" ht="13.8" customHeight="true">
-      <c r="A3" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="12.75" customHeight="true">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="true">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="true">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="12.75" customHeight="true">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>45.45</v>
       </c>
     </row>
-    <row r="5" ht="12.8" customHeight="true">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="12.75" customHeight="true">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>459.987</v>
       </c>
     </row>
-    <row r="6" ht="25.6" customHeight="true">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="25.5" customHeight="true">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>888</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="7" ht="13.8" customHeight="true">
-      <c r="A7" s="7" t="s">
+    <row r="7" ht="12.75" customHeight="true">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
         <v>9</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>505.437</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="true">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="true">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10">
+        <v>45.45</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="true">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="10">
+        <v>7</v>
+      </c>
+      <c r="D10" s="10">
+        <v>459.987</v>
+      </c>
+    </row>
+    <row r="11" ht="25.5" customHeight="true">
+      <c r="A11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10">
+        <v>888</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>